<commit_message>
Rename 'field_type' to 'generate_audio_file' attribute
</commit_message>
<xml_diff>
--- a/test/resources/assets/English_Golden_List.xlsx
+++ b/test/resources/assets/English_Golden_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rino\Workspace\Code\Python\Projects\Anki-Composer\test\resources\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F99B2C-2BBB-4CAA-B0FA-4FC27178AEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7631F1C0-B074-4955-A29E-A20C4EE2AD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19092" yWindow="-4476" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DETAILS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="370">
   <si>
     <t>version</t>
   </si>
@@ -1126,245 +1126,20 @@
     <t>[sound:English_Golden_List.v2_23.3.mp3]</t>
   </si>
   <si>
-    <t>[sound:English_Golden_List.v2_24.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_24.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_24.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_25.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_25.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_25.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_26.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_26.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_26.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_27.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_27.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_27.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_28.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_28.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_28.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_29.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_29.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_29.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_30.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_30.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_30.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_31.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_31.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_31.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_32.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_32.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_32.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_33.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_33.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_33.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_34.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_34.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_34.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_35.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_35.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_35.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_36.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_36.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_36.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_37.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_37.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_37.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_38.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_38.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_38.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_39.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_39.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_39.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_40.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_40.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_40.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_41.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_41.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_41.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_42.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_42.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_42.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_43.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_43.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_43.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_44.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_44.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_44.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_45.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_45.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_45.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_46.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_46.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_46.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_47.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_47.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_47.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_48.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_48.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_48.3.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_49.1.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_49.2.mp3]</t>
-  </si>
-  <si>
-    <t>[sound:English_Golden_List.v2_49.3.mp3]</t>
+    <t>EXAMPLE_3</t>
+  </si>
+  <si>
+    <t>EXAMPLE_2</t>
+  </si>
+  <si>
+    <t>EXAMPLE_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1400,13 +1175,6 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1422,7 +1190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1445,101 +1213,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1559,24 +1237,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1800,13 +1460,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1828,13 +1488,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1842,7 +1502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1858,7 +1518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1866,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1874,7 +1534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1882,7 +1542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1890,7 +1550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1898,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1906,7 +1566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1914,7 +1574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1922,7 +1582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1930,7 +1590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1938,7 +1598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1606,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1954,7 +1614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -1962,7 +1622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
@@ -1970,7 +1630,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1978,7 +1638,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1986,7 +1646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
@@ -1994,7 +1654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
@@ -2002,7 +1662,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
@@ -2026,18 +1686,18 @@
       <selection activeCell="G2" sqref="G2:I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" customWidth="1"/>
-    <col min="4" max="4" width="58.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="58.85546875" customWidth="1"/>
     <col min="5" max="5" width="71" customWidth="1"/>
-    <col min="6" max="6" width="59.44140625" customWidth="1"/>
-    <col min="7" max="9" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" customWidth="1"/>
+    <col min="7" max="9" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -2066,7 +1726,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2095,7 +1755,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2124,7 +1784,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2153,7 +1813,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2182,7 +1842,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2211,7 +1871,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2240,7 +1900,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2269,7 +1929,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2298,7 +1958,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2327,7 +1987,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2356,7 +2016,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2385,7 +2045,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2414,7 +2074,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2443,7 +2103,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2472,7 +2132,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2501,7 +2161,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2530,7 +2190,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2559,7 +2219,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2588,7 +2248,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2617,7 +2277,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2646,7 +2306,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2675,7 +2335,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2704,7 +2364,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2743,24 +2403,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.44140625" customWidth="1"/>
-    <col min="3" max="3" width="65.77734375" customWidth="1"/>
-    <col min="4" max="4" width="65.109375" customWidth="1"/>
-    <col min="5" max="5" width="60.88671875" customWidth="1"/>
-    <col min="6" max="6" width="75" customWidth="1"/>
-    <col min="7" max="9" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" customWidth="1"/>
+    <col min="6" max="6" width="87.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -2771,25 +2430,16 @@
         <v>47</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>369</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>368</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>24</v>
       </c>
@@ -2808,17 +2458,8 @@
       <c r="F2" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>25</v>
       </c>
@@ -2837,17 +2478,8 @@
       <c r="F3" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>26</v>
       </c>
@@ -2866,17 +2498,8 @@
       <c r="F4" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>27</v>
       </c>
@@ -2895,17 +2518,8 @@
       <c r="F5" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>28</v>
       </c>
@@ -2924,17 +2538,8 @@
       <c r="F6" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>29</v>
       </c>
@@ -2953,17 +2558,8 @@
       <c r="F7" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>30</v>
       </c>
@@ -2982,17 +2578,8 @@
       <c r="F8" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>31</v>
       </c>
@@ -3011,17 +2598,8 @@
       <c r="F9" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>389</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>32</v>
       </c>
@@ -3040,17 +2618,8 @@
       <c r="F10" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>33</v>
       </c>
@@ -3069,17 +2638,8 @@
       <c r="F11" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>34</v>
       </c>
@@ -3098,17 +2658,8 @@
       <c r="F12" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>397</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>35</v>
       </c>
@@ -3127,17 +2678,8 @@
       <c r="F13" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>36</v>
       </c>
@@ -3156,17 +2698,8 @@
       <c r="F14" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>37</v>
       </c>
@@ -3185,17 +2718,8 @@
       <c r="F15" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>406</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>38</v>
       </c>
@@ -3214,17 +2738,8 @@
       <c r="F16" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>409</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>39</v>
       </c>
@@ -3243,17 +2758,8 @@
       <c r="F17" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>40</v>
       </c>
@@ -3272,17 +2778,8 @@
       <c r="F18" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>416</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41</v>
       </c>
@@ -3301,17 +2798,8 @@
       <c r="F19" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>42</v>
       </c>
@@ -3330,17 +2818,8 @@
       <c r="F20" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43</v>
       </c>
@@ -3359,17 +2838,8 @@
       <c r="F21" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>44</v>
       </c>
@@ -3388,17 +2858,8 @@
       <c r="F22" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>45</v>
       </c>
@@ -3417,17 +2878,8 @@
       <c r="F23" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>431</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>46</v>
       </c>
@@ -3446,17 +2898,8 @@
       <c r="F24" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>47</v>
       </c>
@@ -3475,17 +2918,8 @@
       <c r="F25" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>48</v>
       </c>
@@ -3504,17 +2938,8 @@
       <c r="F26" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>440</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>49</v>
       </c>
@@ -3532,15 +2957,6 @@
       </c>
       <c r="F27" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>